<commit_message>
school upload down load done
</commit_message>
<xml_diff>
--- a/uploads/schools.xlsx
+++ b/uploads/schools.xlsx
@@ -1,46 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megwu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lincoln Uni\Computing\639\pj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D22B83B-D162-4134-87A5-97855AEE1374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2021 active list" sheetId="1" r:id="rId1"/>
+    <sheet name="2021 active list " sheetId="3" r:id="rId1"/>
     <sheet name="Waiting list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -148,22 +140,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Returning Number</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Max Number 2021</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Confirmed Number</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coordinator ID</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Portal </t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -192,29 +168,64 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>NA</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <t>Coordinator Name</t>
+  </si>
+  <si>
+    <t>Coordinator eMail</t>
+  </si>
+  <si>
+    <t>Returning (Last year)</t>
+  </si>
+  <si>
+    <t>Max Number(Current Year)</t>
+  </si>
+  <si>
+    <t>Current Year</t>
+  </si>
+  <si>
+    <t>Total(Current Year)</t>
+  </si>
+  <si>
+    <t>Requested Number(Current Year)</t>
+  </si>
+  <si>
+    <t>Confirmed Number(Current Year)</t>
+  </si>
+  <si>
+    <t>Total(Previous)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam </t>
+  </si>
+  <si>
+    <t>Sam@ccsc.school.nz</t>
+  </si>
+  <si>
+    <t>Donna</t>
+  </si>
+  <si>
+    <t>Donna@ccc.school.nz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="164" formatCode="0_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -222,7 +233,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -230,7 +241,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -238,7 +249,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -246,28 +257,34 @@
       <b/>
       <sz val="20"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -324,7 +341,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -372,20 +389,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -701,30 +724,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9A5B8A-BEBC-4007-ADD0-E8216ED9EA4F}">
+  <dimension ref="A1:W267"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="22"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="17" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="10" width="24.1640625" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="22" customWidth="1"/>
-    <col min="14" max="15" width="17.1640625" customWidth="1"/>
-    <col min="16" max="17" width="21.1640625" customWidth="1"/>
-    <col min="18" max="18" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="21"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="13" width="17.109375" customWidth="1"/>
+    <col min="14" max="15" width="21.109375" customWidth="1"/>
+    <col min="16" max="16" width="39.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="18" max="18" width="19" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="16" customFormat="1">
       <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
@@ -743,45 +773,60 @@
       <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="21">
+      <c r="Q1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="24">
         <v>1046</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -799,45 +844,55 @@
       <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="6">
+        <v>44242</v>
+      </c>
+      <c r="J2" s="6">
+        <v>44242</v>
+      </c>
+      <c r="K2" s="6">
+        <v>44270</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>2021</v>
+      </c>
+      <c r="R2" s="19">
         <v>8</v>
       </c>
-      <c r="H2" s="4">
+      <c r="S2" s="4">
         <v>40</v>
       </c>
-      <c r="I2" s="5">
+      <c r="T2" s="5">
         <v>25</v>
       </c>
-      <c r="J2" s="5">
-        <v>1010</v>
-      </c>
-      <c r="K2" s="6">
-        <v>44242</v>
-      </c>
-      <c r="L2" s="6">
-        <v>44242</v>
-      </c>
-      <c r="M2" s="6">
-        <v>44270</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="21">
+      <c r="U2" s="5">
+        <v>25</v>
+      </c>
+      <c r="V2" s="22"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="24">
         <v>1047</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -855,49 +910,59 @@
       <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="6">
+        <v>44242</v>
+      </c>
+      <c r="J3" s="6">
+        <v>44243</v>
+      </c>
+      <c r="K3" s="6">
+        <v>44278</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="R3" s="19">
         <v>0</v>
       </c>
-      <c r="H3" s="4">
+      <c r="S3" s="4">
         <v>30</v>
       </c>
-      <c r="I3" s="5">
+      <c r="T3" s="5">
         <v>39</v>
       </c>
-      <c r="J3" s="5">
-        <v>1011</v>
-      </c>
-      <c r="K3" s="6">
-        <v>44242</v>
-      </c>
-      <c r="L3" s="6">
-        <v>44243</v>
-      </c>
-      <c r="M3" s="6">
-        <v>44278</v>
-      </c>
-      <c r="N3" s="6" t="s">
+      <c r="U3" s="5">
+        <v>39</v>
+      </c>
+      <c r="V3" s="22"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="24">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
-        <v>48</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -911,49 +976,59 @@
       <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="6">
+        <v>44242</v>
+      </c>
+      <c r="J4" s="6">
+        <v>44243</v>
+      </c>
+      <c r="K4" s="6">
+        <v>44278</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="R4" s="19">
         <v>2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="S4" s="4">
         <v>30</v>
       </c>
-      <c r="I4" s="5">
+      <c r="T4" s="5">
         <v>39</v>
       </c>
-      <c r="J4" s="5">
-        <v>1011</v>
-      </c>
-      <c r="K4" s="6">
-        <v>44242</v>
-      </c>
-      <c r="L4" s="6">
-        <v>44243</v>
-      </c>
-      <c r="M4" s="6">
-        <v>44278</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="21">
+      <c r="U4" s="5">
+        <v>39</v>
+      </c>
+      <c r="V4" s="22"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="24">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -967,72 +1042,868 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
+        <v>44243</v>
+      </c>
+      <c r="K5" s="6">
+        <v>44278</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>2021</v>
+      </c>
+      <c r="R5" s="19">
         <v>2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="S5" s="4">
         <v>30</v>
       </c>
-      <c r="I5" s="5">
+      <c r="T5" s="5">
         <v>39</v>
       </c>
-      <c r="J5" s="5">
-        <v>1011</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" s="6">
-        <v>44243</v>
-      </c>
-      <c r="M5" s="6">
-        <v>44278</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="F9" s="2"/>
+      <c r="U5" s="5">
+        <v>39</v>
+      </c>
+      <c r="V5" s="22"/>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" s="24"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="24"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="24"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="24"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="24"/>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="24"/>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="24"/>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" s="24"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="24"/>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="24"/>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="24"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="24"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="24"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="24"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="24"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="24"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="24"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="24"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="24"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="24"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="24"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="24"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="24"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="24"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="24"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="24"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="24"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="24"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="24"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="24"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="24"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="24"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="24"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="24"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="24"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="24"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="24"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="24"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="24"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="24"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="24"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="24"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="24"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="24"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="24"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="24"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="24"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="24"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="24"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="24"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="24"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="24"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="24"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="24"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="24"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="24"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="24"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="24"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="24"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="24"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="24"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="24"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="24"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="24"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="24"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="24"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="24"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="24"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="24"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="24"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="24"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="24"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="24"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="24"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="24"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="24"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="24"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="24"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="24"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="24"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="24"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="24"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="24"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="24"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="24"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="24"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="24"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="24"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="24"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="24"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="24"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="24"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="24"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="24"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="24"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="24"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="24"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="24"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="24"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="24"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="24"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="24"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="24"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="24"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="24"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="24"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="24"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="24"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="24"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="24"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="24"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="24"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="24"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="24"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="24"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="24"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="24"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="24"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="24"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="24"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="24"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="24"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="24"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="24"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="24"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="24"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="24"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="24"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="24"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="24"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="24"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="24"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="24"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="24"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="24"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="24"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="24"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="24"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="24"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="24"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="24"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="24"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="24"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="24"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="24"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="24"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="24"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="24"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="24"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="24"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="24"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="24"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="24"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="24"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="24"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="24"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="24"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="24"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="24"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="24"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="24"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="24"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="24"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="24"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="24"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="24"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="24"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="24"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="24"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="24"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="24"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="24"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="24"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="24"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="24"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="24"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="24"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="24"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="24"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="24"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="24"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="24"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="24"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="24"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="24"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="24"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="24"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="24"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="24"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="24"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="24"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="24"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="24"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="24"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="24"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="24"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="24"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="24"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="24"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="24"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="24"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="24"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="24"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="24"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="24"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="24"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="24"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="24"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="24"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="24"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="24"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="24"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="24"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="24"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="24"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="24"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="24"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="24"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="24"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="24"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="24"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="24"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="24"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="24"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="24"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="24"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="24"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="24"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="24"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="24"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="24"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="24"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="24"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="24"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="24"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="24"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="24"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="24"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="24"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="24"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="24"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="24"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="24"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="24"/>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" s="24"/>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" s="24"/>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" s="24"/>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" s="24"/>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" s="24"/>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" s="24"/>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" s="24"/>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" s="24"/>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" s="24"/>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" s="24"/>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" s="24"/>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" s="24"/>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" s="24"/>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" s="24"/>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" s="24"/>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" s="24"/>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" s="24"/>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" s="24"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{2F762023-D8B2-47D8-A6E5-DFF3CCA2C130}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{39E84696-915E-40B1-8206-49B289DB7334}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{64D30B9F-789C-453E-B718-D0C38358FE6B}"/>
+    <hyperlink ref="H2" r:id="rId4" xr:uid="{6F29AE53-BCFE-4950-A40E-D7C06C368D6C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="25.8">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -1042,7 +1913,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1083,7 +1954,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -1107,7 +1978,7 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>